<commit_message>
Revised term project rubric
</commit_message>
<xml_diff>
--- a/TermProject/TermProjectRubric-CIS195.xlsx
+++ b/TermProject/TermProjectRubric-CIS195.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\TermProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1AD61-76CC-4C40-9348-3E7027CA9C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1DFE6C-D15F-294F-B5BD-8563FC426864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="2664" windowWidth="11760" windowHeight="12204" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="10620" yWindow="500" windowWidth="18180" windowHeight="16480" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Student Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Possible</t>
   </si>
@@ -113,6 +104,9 @@
   </si>
   <si>
     <t>Each page has section, article and header</t>
+  </si>
+  <si>
+    <t>Points</t>
   </si>
 </sst>
 </file>
@@ -212,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -220,11 +214,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -255,6 +258,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,267 +577,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:B31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
-    <col min="2" max="3" width="11.19921875" style="10"/>
+    <col min="2" max="2" width="8.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="12">
-        <v>10</v>
-      </c>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="12">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="12">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="12">
-        <v>5</v>
-      </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="12">
-        <v>10</v>
-      </c>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="12">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="12">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="12">
-        <v>3</v>
-      </c>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="13">
         <f>SUM(B4:B12)</f>
-        <v>55</v>
-      </c>
-      <c r="C13" s="13"/>
+        <v>135</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="12">
-        <v>5</v>
-      </c>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="12">
-        <v>5</v>
-      </c>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="17">
-        <v>5</v>
-      </c>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="12">
-        <v>2</v>
-      </c>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="12">
-        <v>3</v>
-      </c>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="12">
-        <v>3</v>
-      </c>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="13">
         <f>SUM(B16:B21)</f>
-        <v>23</v>
-      </c>
-      <c r="C22" s="13"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="12">
-        <v>5</v>
-      </c>
-      <c r="C25" s="12"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="12">
-        <v>15</v>
-      </c>
-      <c r="C26" s="12"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="13">
         <f>SUM(B25:B26)</f>
-        <v>20</v>
-      </c>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="12">
-        <v>2</v>
-      </c>
-      <c r="C29" s="12"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="15">
         <f>SUM(B13,B22,B27,B29)</f>
-        <v>100</v>
-      </c>
-      <c r="C31" s="15"/>
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -845,17 +824,17 @@
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
@@ -864,14 +843,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -882,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -893,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -904,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -915,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -926,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -937,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -948,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -959,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -970,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>3</v>
       </c>
@@ -983,18 +962,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
@@ -1005,7 +984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -1060,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>3</v>
       </c>
@@ -1073,19 +1052,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>3</v>
       </c>
@@ -1120,12 +1099,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>20</v>
       </c>
@@ -1136,12 +1115,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>